<commit_message>
Remade the plots and did small bugfixes
</commit_message>
<xml_diff>
--- a/data2.xlsx
+++ b/data2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documenten\GitHub\weather-balloon-alternative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAB992F-6CAF-43AE-8E70-C631D31D0149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642CD806-ABA5-442E-8261-842EBA4BBCB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -238,9 +238,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -273,7 +270,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -281,7 +277,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -303,16 +298,17 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,13 +592,20 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -619,376 +622,376 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="40">
+      <c r="A2" s="38">
         <v>6</v>
       </c>
-      <c r="B2" s="4">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4">
-        <v>5</v>
-      </c>
-      <c r="D2" s="6">
+      <c r="B2" s="3">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="38">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7">
+        <v>5</v>
+      </c>
+      <c r="C3" s="7">
+        <v>5</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="38">
+        <v>5</v>
+      </c>
+      <c r="B4" s="12">
+        <v>2</v>
+      </c>
+      <c r="C4" s="13">
+        <v>3</v>
+      </c>
+      <c r="D4" s="14">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="38">
+        <v>20</v>
+      </c>
+      <c r="B5" s="7">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7">
+        <v>5</v>
+      </c>
+      <c r="D5" s="37">
+        <v>0</v>
+      </c>
+      <c r="E5" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="38">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7">
+        <v>5</v>
+      </c>
+      <c r="D6" s="16">
+        <v>2</v>
+      </c>
+      <c r="E6" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="38">
         <v>1</v>
       </c>
-      <c r="E2" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="B7" s="9">
+        <v>2</v>
+      </c>
+      <c r="C7" s="15">
+        <v>5</v>
+      </c>
+      <c r="D7" s="9">
+        <v>2</v>
+      </c>
+      <c r="E7" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="38">
+        <v>5</v>
+      </c>
+      <c r="B8" s="41">
+        <v>0</v>
+      </c>
+      <c r="C8" s="17">
+        <v>2</v>
+      </c>
+      <c r="D8" s="18">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="38">
+        <v>15</v>
+      </c>
+      <c r="B9" s="41">
+        <v>0</v>
+      </c>
+      <c r="C9" s="19">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4">
+        <v>3</v>
+      </c>
+      <c r="E9" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="38">
+        <v>12</v>
+      </c>
+      <c r="B10" s="12">
+        <v>2</v>
+      </c>
+      <c r="C10" s="7">
+        <v>5</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2</v>
+      </c>
+      <c r="E10" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="38">
+        <v>16</v>
+      </c>
+      <c r="B11" s="16">
+        <v>2</v>
+      </c>
+      <c r="C11" s="20">
+        <v>3</v>
+      </c>
+      <c r="D11" s="18">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="38">
+        <v>7</v>
+      </c>
+      <c r="B12" s="39">
+        <v>0</v>
+      </c>
+      <c r="C12" s="22">
+        <v>2</v>
+      </c>
+      <c r="D12" s="11">
+        <v>5</v>
+      </c>
+      <c r="E12" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="38">
+        <v>5</v>
+      </c>
+      <c r="B13" s="22">
+        <v>2</v>
+      </c>
+      <c r="C13" s="22">
+        <v>2</v>
+      </c>
+      <c r="D13" s="11">
+        <v>5</v>
+      </c>
+      <c r="E13" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="38">
+        <v>16</v>
+      </c>
+      <c r="B14" s="21">
+        <v>0</v>
+      </c>
+      <c r="C14" s="13">
+        <v>3</v>
+      </c>
+      <c r="D14" s="14">
+        <v>3</v>
+      </c>
+      <c r="E14" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="40">
+        <v>2</v>
+      </c>
+      <c r="B15" s="23">
+        <v>0</v>
+      </c>
+      <c r="C15" s="24">
+        <v>2</v>
+      </c>
+      <c r="D15" s="11">
+        <v>5</v>
+      </c>
+      <c r="E15" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="38">
+        <v>20</v>
+      </c>
+      <c r="B16" s="21">
+        <v>0</v>
+      </c>
+      <c r="C16" s="12">
+        <v>2</v>
+      </c>
+      <c r="D16" s="26">
+        <v>5</v>
+      </c>
+      <c r="E16" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="38">
+        <v>10</v>
+      </c>
+      <c r="B17" s="27">
+        <v>0</v>
+      </c>
+      <c r="C17" s="28">
+        <v>2</v>
+      </c>
+      <c r="D17" s="18">
+        <v>5</v>
+      </c>
+      <c r="E17" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="38">
+        <v>20</v>
+      </c>
+      <c r="B18" s="12">
+        <v>2</v>
+      </c>
+      <c r="C18" s="7">
+        <v>5</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3</v>
+      </c>
+      <c r="E18" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="38">
+        <v>8</v>
+      </c>
+      <c r="B19" s="29">
+        <v>0</v>
+      </c>
+      <c r="C19" s="9">
+        <v>2</v>
+      </c>
+      <c r="D19" s="11">
+        <v>5</v>
+      </c>
+      <c r="E19" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="38">
+        <v>15</v>
+      </c>
+      <c r="B20" s="21">
+        <v>0</v>
+      </c>
+      <c r="C20" s="21">
+        <v>0</v>
+      </c>
+      <c r="D20" s="14">
+        <v>3</v>
+      </c>
+      <c r="E20" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="38">
         <v>4</v>
       </c>
-      <c r="B3" s="8">
-        <v>5</v>
-      </c>
-      <c r="C3" s="8">
-        <v>5</v>
-      </c>
-      <c r="D3" s="9">
-        <v>2</v>
-      </c>
-      <c r="E3" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>5</v>
-      </c>
-      <c r="B4" s="13">
-        <v>2</v>
-      </c>
-      <c r="C4" s="14">
-        <v>3</v>
-      </c>
-      <c r="D4" s="15">
-        <v>3</v>
-      </c>
-      <c r="E4" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>20</v>
-      </c>
-      <c r="B5" s="8">
-        <v>5</v>
-      </c>
-      <c r="C5" s="8">
-        <v>5</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>3</v>
-      </c>
-      <c r="B6" s="8">
-        <v>5</v>
-      </c>
-      <c r="C6" s="8">
-        <v>5</v>
-      </c>
-      <c r="D6" s="17">
-        <v>2</v>
-      </c>
-      <c r="E6" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>1</v>
-      </c>
-      <c r="B7" s="10">
-        <v>2</v>
-      </c>
-      <c r="C7" s="16">
-        <v>5</v>
-      </c>
-      <c r="D7" s="10">
-        <v>2</v>
-      </c>
-      <c r="E7" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>5</v>
-      </c>
-      <c r="B8" s="18">
-        <v>0</v>
-      </c>
-      <c r="C8" s="19">
-        <v>2</v>
-      </c>
-      <c r="D8" s="20">
-        <v>5</v>
-      </c>
-      <c r="E8" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>15</v>
-      </c>
-      <c r="B9" s="18">
-        <v>0</v>
-      </c>
-      <c r="C9" s="21">
-        <v>3</v>
-      </c>
-      <c r="D9" s="5">
-        <v>3</v>
-      </c>
-      <c r="E9" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>12</v>
-      </c>
-      <c r="B10" s="13">
-        <v>2</v>
-      </c>
-      <c r="C10" s="8">
-        <v>5</v>
-      </c>
-      <c r="D10" s="6">
-        <v>2</v>
-      </c>
-      <c r="E10" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="B21" s="22">
+        <v>2</v>
+      </c>
+      <c r="C21" s="22">
+        <v>2</v>
+      </c>
+      <c r="D21" s="30">
+        <v>5</v>
+      </c>
+      <c r="E21" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="38">
+        <v>10</v>
+      </c>
+      <c r="B22" s="32">
+        <v>2</v>
+      </c>
+      <c r="C22" s="32">
+        <v>2</v>
+      </c>
+      <c r="D22" s="31">
+        <v>5</v>
+      </c>
+      <c r="E22" s="33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="38">
         <v>16</v>
       </c>
-      <c r="B11" s="17">
-        <v>2</v>
-      </c>
-      <c r="C11" s="22">
-        <v>3</v>
-      </c>
-      <c r="D11" s="20">
-        <v>5</v>
-      </c>
-      <c r="E11" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>7</v>
-      </c>
-      <c r="B12" s="24">
-        <v>0</v>
-      </c>
-      <c r="C12" s="25">
-        <v>2</v>
-      </c>
-      <c r="D12" s="12">
-        <v>5</v>
-      </c>
-      <c r="E12" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>5</v>
-      </c>
-      <c r="B13" s="25">
-        <v>2</v>
-      </c>
-      <c r="C13" s="25">
-        <v>2</v>
-      </c>
-      <c r="D13" s="12">
-        <v>5</v>
-      </c>
-      <c r="E13" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>16</v>
-      </c>
-      <c r="B14" s="23">
-        <v>0</v>
-      </c>
-      <c r="C14" s="14">
-        <v>3</v>
-      </c>
-      <c r="D14" s="15">
-        <v>3</v>
-      </c>
-      <c r="E14" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="41">
-        <v>2</v>
-      </c>
-      <c r="B15" s="26">
-        <v>0</v>
-      </c>
-      <c r="C15" s="27">
-        <v>2</v>
-      </c>
-      <c r="D15" s="12">
-        <v>5</v>
-      </c>
-      <c r="E15" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>20</v>
-      </c>
-      <c r="B16" s="23">
-        <v>0</v>
-      </c>
-      <c r="C16" s="13">
-        <v>2</v>
-      </c>
-      <c r="D16" s="29">
-        <v>5</v>
-      </c>
-      <c r="E16" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
-        <v>10</v>
-      </c>
-      <c r="B17" s="30">
-        <v>0</v>
-      </c>
-      <c r="C17" s="31">
-        <v>2</v>
-      </c>
-      <c r="D17" s="20">
-        <v>5</v>
-      </c>
-      <c r="E17" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
-        <v>20</v>
-      </c>
-      <c r="B18" s="13">
-        <v>2</v>
-      </c>
-      <c r="C18" s="8">
-        <v>5</v>
-      </c>
-      <c r="D18" s="5">
-        <v>3</v>
-      </c>
-      <c r="E18" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
-        <v>8</v>
-      </c>
-      <c r="B19" s="32">
-        <v>0</v>
-      </c>
-      <c r="C19" s="10">
-        <v>2</v>
-      </c>
-      <c r="D19" s="12">
-        <v>5</v>
-      </c>
-      <c r="E19" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
-        <v>15</v>
-      </c>
-      <c r="B20" s="23">
-        <v>0</v>
-      </c>
-      <c r="C20" s="23">
-        <v>0</v>
-      </c>
-      <c r="D20" s="15">
-        <v>3</v>
-      </c>
-      <c r="E20" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
-        <v>4</v>
-      </c>
-      <c r="B21" s="24">
-        <v>0</v>
-      </c>
-      <c r="C21" s="25">
-        <v>2</v>
-      </c>
-      <c r="D21" s="33">
-        <v>5</v>
-      </c>
-      <c r="E21" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
-        <v>10</v>
-      </c>
-      <c r="B22" s="36">
-        <v>2</v>
-      </c>
-      <c r="C22" s="36">
-        <v>2</v>
-      </c>
-      <c r="D22" s="35">
-        <v>5</v>
-      </c>
-      <c r="E22" s="37">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
-        <v>16</v>
-      </c>
       <c r="B23" s="34">
-        <v>2</v>
-      </c>
-      <c r="C23" s="38">
-        <v>0</v>
-      </c>
-      <c r="D23" s="39">
-        <v>3</v>
-      </c>
-      <c r="E23" s="39">
+        <v>0</v>
+      </c>
+      <c r="C23" s="34">
+        <v>0</v>
+      </c>
+      <c r="D23" s="35">
+        <v>3</v>
+      </c>
+      <c r="E23" s="35">
         <v>3</v>
       </c>
     </row>

</xml_diff>